<commit_message>
adding data sets info
</commit_message>
<xml_diff>
--- a/Assignment1/Assignment1_Rough.xlsx
+++ b/Assignment1/Assignment1_Rough.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lakshmi Priyanka\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\599Git\599ProjectWork\Assignment1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="50">
   <si>
     <t>https://catalog.data.gov/dataset/national-flood-hazard-layer-nfhl</t>
   </si>
@@ -90,6 +90,91 @@
   </si>
   <si>
     <t>Mental Health</t>
+  </si>
+  <si>
+    <t>Data type</t>
+  </si>
+  <si>
+    <t>MIME Type</t>
+  </si>
+  <si>
+    <t>https://catalog.data.gov/dataset/aerial-photos-of-the-1940s</t>
+  </si>
+  <si>
+    <t>https://catalog.data.gov/dataset/h11188-nos-hydrographic-survey-admiralty-inlet-and-port-townsend-washing-11-05</t>
+  </si>
+  <si>
+    <t>Image</t>
+  </si>
+  <si>
+    <t>Overlap</t>
+  </si>
+  <si>
+    <t>8 years</t>
+  </si>
+  <si>
+    <t>29 years</t>
+  </si>
+  <si>
+    <t>23 years</t>
+  </si>
+  <si>
+    <t>88 years</t>
+  </si>
+  <si>
+    <t>full overlap</t>
+  </si>
+  <si>
+    <t>json, text</t>
+  </si>
+  <si>
+    <t>KML, KMZ</t>
+  </si>
+  <si>
+    <t>Several split files</t>
+  </si>
+  <si>
+    <t>12 years</t>
+  </si>
+  <si>
+    <t>Single CSV</t>
+  </si>
+  <si>
+    <t>Text\csv</t>
+  </si>
+  <si>
+    <t>Applciation\HTML</t>
+  </si>
+  <si>
+    <t>text\csv</t>
+  </si>
+  <si>
+    <t>Application/xml
+SHP file (Application/octet-stream)</t>
+  </si>
+  <si>
+    <t>https://catalog.data.gov/dataset/deaths-in-122-u-s-cities-1962-2016-122-cities-mortality-reporting-system</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Json, </t>
+  </si>
+  <si>
+    <t>https://catalog.data.gov/dataset/waofm-april-1-population-by-state-county-and-city-1990-to-present-22a1f</t>
+  </si>
+  <si>
+    <t>17 years</t>
+  </si>
+  <si>
+    <t>State wide</t>
+  </si>
+  <si>
+    <t>https://catalog.data.gov/dataset/drug-poisoning-mortality-by-county-united-states</t>
+  </si>
+  <si>
+    <t>https://catalog.data.gov/dataset/behavioral-risk-factor-data-health-related-quality-of-life-hrqol-76ea6</t>
+  </si>
+  <si>
+    <t>https://catalog.data.gov/dataset/infant-and-neonatal-mortality-rates-united-states-1915-2013</t>
   </si>
 </sst>
 </file>
@@ -121,12 +206,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -142,10 +233,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -461,35 +572,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="139.90625" customWidth="1"/>
+    <col min="1" max="1" width="97.36328125" customWidth="1"/>
+    <col min="4" max="4" width="12.54296875" customWidth="1"/>
+    <col min="6" max="6" width="10.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="D1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B3">
@@ -499,8 +621,8 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="6" t="s">
         <v>3</v>
       </c>
       <c r="B4">
@@ -509,9 +631,15 @@
       <c r="C4">
         <v>2017</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="D4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="6" t="s">
         <v>2</v>
       </c>
       <c r="B5">
@@ -520,9 +648,15 @@
       <c r="C5">
         <v>2010</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="D5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B6" t="s">
@@ -532,13 +666,13 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+    <row r="7" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B8" t="s">
@@ -548,8 +682,8 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B9">
@@ -558,9 +692,15 @@
       <c r="C9">
         <v>2017</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+      <c r="D9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" s="6" t="s">
         <v>14</v>
       </c>
       <c r="B10">
@@ -569,48 +709,172 @@
       <c r="C10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+      <c r="D10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" t="s">
+        <v>35</v>
+      </c>
+      <c r="F10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11">
+        <v>1995</v>
+      </c>
+      <c r="C11">
+        <v>2009</v>
+      </c>
+      <c r="D11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B11">
+      <c r="B12">
         <v>1870</v>
       </c>
-      <c r="C11">
+      <c r="C12">
         <v>2015</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+      <c r="D12" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E13" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D14" t="s">
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16">
+        <v>1940</v>
+      </c>
+      <c r="C16">
+        <v>1940</v>
+      </c>
+      <c r="D16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19">
+        <v>1962</v>
+      </c>
+      <c r="C19">
+        <v>2016</v>
+      </c>
+      <c r="D19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>44</v>
+      </c>
+      <c r="B20">
+        <v>1990</v>
+      </c>
+      <c r="C20" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" t="s">
+        <v>45</v>
+      </c>
+      <c r="G20" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A21" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A22" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B22" s="9">
+        <v>1993</v>
+      </c>
+      <c r="C22" s="9">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24">
+        <v>1915</v>
+      </c>
+      <c r="C24">
+        <v>2013</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A4" r:id="rId1"/>
     <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A5" r:id="rId3"/>
+    <hyperlink ref="A9" r:id="rId4"/>
+    <hyperlink ref="A11" r:id="rId5"/>
+    <hyperlink ref="A10" r:id="rId6"/>
+    <hyperlink ref="A12" r:id="rId7"/>
+    <hyperlink ref="A13" r:id="rId8"/>
+    <hyperlink ref="A22" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
all files related to census data set
</commit_message>
<xml_diff>
--- a/Assignment1/Assignment1_Rough.xlsx
+++ b/Assignment1/Assignment1_Rough.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4100"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4100" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Datasets Selection" sheetId="1" r:id="rId1"/>
+    <sheet name="CensusByYear" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="72">
   <si>
     <t>https://catalog.data.gov/dataset/national-flood-hazard-layer-nfhl</t>
   </si>
@@ -175,13 +176,79 @@
   </si>
   <si>
     <t>https://catalog.data.gov/dataset/infant-and-neonatal-mortality-rates-united-states-1915-2013</t>
+  </si>
+  <si>
+    <t>https://catalog.data.gov/dataset/continental-united-states-hurricane-strikes-1950-2012</t>
+  </si>
+  <si>
+    <t>Pdf</t>
+  </si>
+  <si>
+    <t>https://catalog.data.gov/dataset/us-monthly-pilot-balloon-observations</t>
+  </si>
+  <si>
+    <t>3 Columns</t>
+  </si>
+  <si>
+    <t>Geographical Area</t>
+  </si>
+  <si>
+    <t>Population</t>
+  </si>
+  <si>
+    <t>Housing units</t>
+  </si>
+  <si>
+    <t>Area in square miles</t>
+  </si>
+  <si>
+    <t>Density per square mile of land area</t>
+  </si>
+  <si>
+    <t>Total area</t>
+  </si>
+  <si>
+    <t>Water area</t>
+  </si>
+  <si>
+    <t>Land area</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>Los Angeles County, California</t>
+  </si>
+  <si>
+    <t>Cook County, Illinois</t>
+  </si>
+  <si>
+    <t>Harris County, Texas</t>
+  </si>
+  <si>
+    <t>Maricopa County, Arizona</t>
+  </si>
+  <si>
+    <t>Orange County, California</t>
+  </si>
+  <si>
+    <t>San Diego County, California</t>
+  </si>
+  <si>
+    <t>Kings County, New York</t>
+  </si>
+  <si>
+    <t>Miami-Dade County, Florida</t>
+  </si>
+  <si>
+    <t>Queens County, New York</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -205,8 +272,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="6"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -219,8 +299,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEAE8E6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -228,12 +320,106 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFAAAAAA"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FFAAAAAA"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFAAAAAA"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFAAAAAA"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFAAAAAA"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFAAAAAA"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFAAAAAA"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFAAAAAA"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFAAAAAA"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFAAAAAA"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFAAAAAA"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFAAAAAA"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FFAAAAAA"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFAAAAAA"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FFAAAAAA"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFAAAAAA"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFAAAAAA"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFAAAAAA"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFAAAAAA"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -257,6 +443,91 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -572,20 +843,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="97.36328125" customWidth="1"/>
-    <col min="4" max="4" width="12.54296875" customWidth="1"/>
-    <col min="6" max="6" width="10.6328125" customWidth="1"/>
+    <col min="4" max="5" width="12.54296875" customWidth="1"/>
+    <col min="7" max="7" width="10.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -599,18 +870,21 @@
         <v>23</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -621,7 +895,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
         <v>3</v>
       </c>
@@ -634,11 +908,11 @@
       <c r="D4" t="s">
         <v>33</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
         <v>2</v>
       </c>
@@ -651,11 +925,11 @@
       <c r="D5" t="s">
         <v>34</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -666,12 +940,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>11</v>
       </c>
@@ -682,7 +956,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>13</v>
       </c>
@@ -695,11 +969,11 @@
       <c r="D9" t="s">
         <v>40</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="6" t="s">
         <v>14</v>
       </c>
@@ -712,14 +986,14 @@
       <c r="D10" t="s">
         <v>39</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>35</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
         <v>14</v>
       </c>
@@ -732,14 +1006,14 @@
       <c r="D11" t="s">
         <v>38</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>37</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A12" s="6" t="s">
         <v>15</v>
       </c>
@@ -752,38 +1026,40 @@
       <c r="D12" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F12" t="s">
+      <c r="E12" s="3"/>
+      <c r="G12" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="8" t="s">
         <v>18</v>
       </c>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
-      <c r="E15" s="7" t="s">
+      <c r="E15" s="7"/>
+      <c r="F15" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -797,12 +1073,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>42</v>
       </c>
@@ -816,7 +1092,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>44</v>
       </c>
@@ -826,21 +1102,21 @@
       <c r="C20" t="s">
         <v>9</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>45</v>
       </c>
-      <c r="G20" t="s">
+      <c r="H20" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" s="9" t="s">
         <v>47</v>
       </c>
       <c r="B21" s="9"/>
       <c r="C21" s="9"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" s="10" t="s">
         <v>48</v>
       </c>
@@ -851,7 +1127,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>49</v>
       </c>
@@ -860,6 +1136,31 @@
       </c>
       <c r="C24">
         <v>2013</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26">
+        <v>1950</v>
+      </c>
+      <c r="C26">
+        <v>2012</v>
+      </c>
+      <c r="D26" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>52</v>
+      </c>
+      <c r="B28">
+        <v>1918</v>
+      </c>
+      <c r="C28">
+        <v>1960</v>
       </c>
     </row>
   </sheetData>
@@ -877,4 +1178,330 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId10"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="11"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+    </row>
+    <row r="2" spans="1:8" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" s="32"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="H2" s="39"/>
+    </row>
+    <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="35"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="E3" s="36" t="s">
+        <v>60</v>
+      </c>
+      <c r="F3" s="36" t="s">
+        <v>61</v>
+      </c>
+      <c r="G3" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="H3" s="37" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" s="15">
+        <v>281421906</v>
+      </c>
+      <c r="C4" s="15">
+        <v>115904641</v>
+      </c>
+      <c r="D4" s="16">
+        <v>3794083.06</v>
+      </c>
+      <c r="E4" s="16">
+        <v>256644.62</v>
+      </c>
+      <c r="F4" s="16">
+        <v>3537438.44</v>
+      </c>
+      <c r="G4" s="17">
+        <v>79.599999999999994</v>
+      </c>
+      <c r="H4" s="18">
+        <v>32.799999999999997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="24" x14ac:dyDescent="0.35">
+      <c r="A5" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" s="20">
+        <v>9519338</v>
+      </c>
+      <c r="C5" s="20">
+        <v>3270909</v>
+      </c>
+      <c r="D5" s="21">
+        <v>4752.32</v>
+      </c>
+      <c r="E5" s="22">
+        <v>691.45</v>
+      </c>
+      <c r="F5" s="21">
+        <v>4060.87</v>
+      </c>
+      <c r="G5" s="21">
+        <v>2344.1999999999998</v>
+      </c>
+      <c r="H5" s="23">
+        <v>805.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="16" x14ac:dyDescent="0.35">
+      <c r="A6" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" s="25">
+        <v>5376741</v>
+      </c>
+      <c r="C6" s="25">
+        <v>2096121</v>
+      </c>
+      <c r="D6" s="26">
+        <v>1635.04</v>
+      </c>
+      <c r="E6" s="27">
+        <v>689.36</v>
+      </c>
+      <c r="F6" s="27">
+        <v>945.68</v>
+      </c>
+      <c r="G6" s="26">
+        <v>5685.6</v>
+      </c>
+      <c r="H6" s="28">
+        <v>2216.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="24" x14ac:dyDescent="0.35">
+      <c r="A7" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="B7" s="20">
+        <v>3400578</v>
+      </c>
+      <c r="C7" s="20">
+        <v>1298130</v>
+      </c>
+      <c r="D7" s="21">
+        <v>1777.69</v>
+      </c>
+      <c r="E7" s="22">
+        <v>48.87</v>
+      </c>
+      <c r="F7" s="21">
+        <v>1728.83</v>
+      </c>
+      <c r="G7" s="21">
+        <v>1967</v>
+      </c>
+      <c r="H7" s="23">
+        <v>750.9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="24" x14ac:dyDescent="0.35">
+      <c r="A8" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="B8" s="25">
+        <v>3072149</v>
+      </c>
+      <c r="C8" s="25">
+        <v>1250231</v>
+      </c>
+      <c r="D8" s="26">
+        <v>9224.27</v>
+      </c>
+      <c r="E8" s="27">
+        <v>21.13</v>
+      </c>
+      <c r="F8" s="26">
+        <v>9203.14</v>
+      </c>
+      <c r="G8" s="27">
+        <v>333.8</v>
+      </c>
+      <c r="H8" s="29">
+        <v>135.80000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="24" x14ac:dyDescent="0.35">
+      <c r="A9" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9" s="20">
+        <v>2846289</v>
+      </c>
+      <c r="C9" s="20">
+        <v>969484</v>
+      </c>
+      <c r="D9" s="22">
+        <v>947.98</v>
+      </c>
+      <c r="E9" s="22">
+        <v>158.57</v>
+      </c>
+      <c r="F9" s="22">
+        <v>789.4</v>
+      </c>
+      <c r="G9" s="21">
+        <v>3605.6</v>
+      </c>
+      <c r="H9" s="30">
+        <v>1228.0999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="24" x14ac:dyDescent="0.35">
+      <c r="A10" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10" s="25">
+        <v>2813833</v>
+      </c>
+      <c r="C10" s="25">
+        <v>1040149</v>
+      </c>
+      <c r="D10" s="26">
+        <v>4525.5200000000004</v>
+      </c>
+      <c r="E10" s="27">
+        <v>325.62</v>
+      </c>
+      <c r="F10" s="26">
+        <v>4199.8900000000003</v>
+      </c>
+      <c r="G10" s="27">
+        <v>670</v>
+      </c>
+      <c r="H10" s="29">
+        <v>247.7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="24" x14ac:dyDescent="0.35">
+      <c r="A11" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11" s="20">
+        <v>2465326</v>
+      </c>
+      <c r="C11" s="20">
+        <v>930866</v>
+      </c>
+      <c r="D11" s="22">
+        <v>96.9</v>
+      </c>
+      <c r="E11" s="22">
+        <v>26.29</v>
+      </c>
+      <c r="F11" s="22">
+        <v>70.61</v>
+      </c>
+      <c r="G11" s="21">
+        <v>34916.6</v>
+      </c>
+      <c r="H11" s="30">
+        <v>13183.9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="24" x14ac:dyDescent="0.35">
+      <c r="A12" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="B12" s="25">
+        <v>2253362</v>
+      </c>
+      <c r="C12" s="25">
+        <v>852278</v>
+      </c>
+      <c r="D12" s="26">
+        <v>2431.2600000000002</v>
+      </c>
+      <c r="E12" s="27">
+        <v>485.19</v>
+      </c>
+      <c r="F12" s="26">
+        <v>1946.06</v>
+      </c>
+      <c r="G12" s="26">
+        <v>1157.9000000000001</v>
+      </c>
+      <c r="H12" s="29">
+        <v>437.9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="24" x14ac:dyDescent="0.35">
+      <c r="A13" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="B13" s="20">
+        <v>2229379</v>
+      </c>
+      <c r="C13" s="20">
+        <v>817250</v>
+      </c>
+      <c r="D13" s="22">
+        <v>178.28</v>
+      </c>
+      <c r="E13" s="22">
+        <v>69.040000000000006</v>
+      </c>
+      <c r="F13" s="22">
+        <v>109.24</v>
+      </c>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="G2:H2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>